<commit_message>
fix rIds to correspond to number of Pivot Cache and not Pivot Tables
</commit_message>
<xml_diff>
--- a/inst/extdata/loadPivotTables.xlsx
+++ b/inst/extdata/loadPivotTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmpivette/Projets_R/Personal_Project/openxlsx/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEAA9DDC-8477-1E44-BA03-DC8E75FC7991}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFC369B-B91E-CF41-905B-7F44309E8291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1040" windowWidth="28040" windowHeight="17440" xr2:uid="{F2E5065D-43FC-7441-BFF6-4F01952EBD72}"/>
+    <workbookView xWindow="1660" yWindow="1040" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{F2E5065D-43FC-7441-BFF6-4F01952EBD72}"/>
   </bookViews>
   <sheets>
     <sheet name="iris" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId6"/>
-    <pivotCache cacheId="18" r:id="rId7"/>
+    <pivotCache cacheId="67" r:id="rId6"/>
+    <pivotCache cacheId="68" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -896,7 +896,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62568726-82EB-3B46-94D7-90705FAB4E38}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{62568726-82EB-3B46-94D7-90705FAB4E38}" name="PivotTable2" cacheId="67" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0">
@@ -1004,7 +1004,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EED7BA66-4DC9-DA40-8A53-FE011051B0D6}" name="PivotTable3" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EED7BA66-4DC9-DA40-8A53-FE011051B0D6}" name="PivotTable3" cacheId="68" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -1093,7 +1093,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A9C97C0-0784-3A49-802E-78C9847F481D}" name="PivotTable4" cacheId="18" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9A9C97C0-0784-3A49-802E-78C9847F481D}" name="PivotTable4" cacheId="68" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1505,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15753262-4B5E-C345-BA84-5AD7FC95C156}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
@@ -2474,8 +2474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0142CF-DD2B-A740-A5DE-7A8308B2EEF3}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2906,7 +2906,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{37BDBC1B-EB4A-B840-AF46-0717EF86621C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>